<commit_message>
Finished generating data for case study 1
</commit_message>
<xml_diff>
--- a/4_example/case_study_1.0/4_additional_plots/nc10.xlsx
+++ b/4_example/case_study_1.0/4_additional_plots/nc10.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tkim333\Documents\GitHub\toPSAil\4_example\plots\plots_case_study_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tkim333\Documents\GitHub\toPSAil\4_example\case_study_1.0\4_additional_plots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6831322-0754-4A2D-A76A-2D08BC2B0C50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A65B3FF9-12E6-4B66-8627-1E14B405ED9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{E71A76A9-1A8C-CE4F-992F-1CEB30169FB9}"/>
   </bookViews>
@@ -399,7 +399,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A2" sqref="A2:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -420,10 +420,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="2">
-        <v>2.5395229872094599E-5</v>
+        <v>2.5373633846282799E-5</v>
       </c>
       <c r="C2" s="2">
-        <v>9.1417606543804897E-5</v>
+        <v>9.1339873099565696E-5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -431,10 +431,10 @@
         <v>8.4666666666666703</v>
       </c>
       <c r="B3" s="2">
-        <v>2.5397019785321301E-5</v>
+        <v>2.53753852060817E-5</v>
       </c>
       <c r="C3" s="2">
-        <v>9.1415816630578201E-5</v>
+        <v>9.1338121739766893E-5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -442,10 +442,10 @@
         <v>16.933333333333302</v>
       </c>
       <c r="B4" s="2">
-        <v>2.5410750273792799E-5</v>
+        <v>2.5388721343385999E-5</v>
       </c>
       <c r="C4" s="2">
-        <v>9.1402086142106594E-5</v>
+        <v>9.13247856024625E-5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -453,10 +453,10 @@
         <v>25.4</v>
       </c>
       <c r="B5" s="2">
-        <v>2.5482749832580502E-5</v>
+        <v>2.5458061208161799E-5</v>
       </c>
       <c r="C5" s="2">
-        <v>9.1330086583318702E-5</v>
+        <v>9.1255445737686595E-5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -464,10 +464,10 @@
         <v>33.866666666666703</v>
       </c>
       <c r="B6" s="2">
-        <v>2.5773810488581599E-5</v>
+        <v>2.57354462076905E-5</v>
       </c>
       <c r="C6" s="2">
-        <v>9.1039025927315599E-5</v>
+        <v>9.0978060738156701E-5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -475,10 +475,10 @@
         <v>42.3333333333333</v>
       </c>
       <c r="B7" s="2">
-        <v>2.6742978502893101E-5</v>
+        <v>2.66479830114691E-5</v>
       </c>
       <c r="C7" s="2">
-        <v>9.0069857912993597E-5</v>
+        <v>9.0065523934370904E-5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -486,10 +486,10 @@
         <v>50.8</v>
       </c>
       <c r="B8" s="2">
-        <v>2.94926130541664E-5</v>
+        <v>2.92066847335379E-5</v>
       </c>
       <c r="C8" s="2">
-        <v>8.7320223361676605E-5</v>
+        <v>8.7506822212269703E-5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -497,10 +497,10 @@
         <v>59.266666666666701</v>
       </c>
       <c r="B9" s="2">
-        <v>3.6110550443337603E-5</v>
+        <v>3.5313787672193602E-5</v>
       </c>
       <c r="C9" s="2">
-        <v>8.0702285972365201E-5</v>
+        <v>8.1399719273495702E-5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -508,10 +508,10 @@
         <v>67.733333333333306</v>
       </c>
       <c r="B10" s="2">
-        <v>4.8950291140604603E-5</v>
+        <v>4.7152616168594397E-5</v>
       </c>
       <c r="C10" s="2">
-        <v>6.78625452747667E-5</v>
+        <v>6.9560890776762605E-5</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -519,10 +519,10 @@
         <v>76.2</v>
       </c>
       <c r="B11" s="2">
-        <v>6.7485498785753906E-5</v>
+        <v>6.4428228194754597E-5</v>
       </c>
       <c r="C11" s="2">
-        <v>4.9327337629168002E-5</v>
+        <v>5.2285278749964603E-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding more case study plots
added plotGasConsHighPresFeed.m
</commit_message>
<xml_diff>
--- a/4_example/case_study_1.0/4_additional_plots/nc10.xlsx
+++ b/4_example/case_study_1.0/4_additional_plots/nc10.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tkim333\Documents\GitHub\toPSAil\4_example\case_study_1.0\4_additional_plots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A65B3FF9-12E6-4B66-8627-1E14B405ED9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156D4479-B160-42A4-9BF7-175D19DAC5EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{E71A76A9-1A8C-CE4F-992F-1CEB30169FB9}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -57,13 +57,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -80,8 +93,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,19 +412,19 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C11"/>
+      <selection sqref="A1:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -419,110 +432,110 @@
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" s="2">
-        <v>2.5373633846282799E-5</v>
-      </c>
-      <c r="C2" s="2">
-        <v>9.1339873099565696E-5</v>
+      <c r="B2" s="1">
+        <v>2.5374630671582701E-5</v>
+      </c>
+      <c r="C2" s="1">
+        <v>9.1343457629429302E-5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>8.4666666666666703</v>
       </c>
-      <c r="B3" s="2">
-        <v>2.53753852060817E-5</v>
-      </c>
-      <c r="C3" s="2">
-        <v>9.1338121739766893E-5</v>
+      <c r="B3" s="1">
+        <v>2.5376393334957401E-5</v>
+      </c>
+      <c r="C3" s="1">
+        <v>9.1341694966054504E-5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>16.933333333333302</v>
       </c>
-      <c r="B4" s="2">
-        <v>2.5388721343385999E-5</v>
-      </c>
-      <c r="C4" s="2">
-        <v>9.13247856024625E-5</v>
+      <c r="B4" s="1">
+        <v>2.53898081249423E-5</v>
+      </c>
+      <c r="C4" s="1">
+        <v>9.1328280176069604E-5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>25.4</v>
       </c>
-      <c r="B5" s="2">
-        <v>2.5458061208161799E-5</v>
-      </c>
-      <c r="C5" s="2">
-        <v>9.1255445737686595E-5</v>
+      <c r="B5" s="1">
+        <v>2.5459524988851201E-5</v>
+      </c>
+      <c r="C5" s="1">
+        <v>9.1258563312160304E-5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>33.866666666666703</v>
       </c>
-      <c r="B6" s="2">
-        <v>2.57354462076905E-5</v>
-      </c>
-      <c r="C6" s="2">
-        <v>9.0978060738156701E-5</v>
+      <c r="B6" s="1">
+        <v>2.5738265450367999E-5</v>
+      </c>
+      <c r="C6" s="1">
+        <v>9.0979822850641802E-5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>42.3333333333333</v>
       </c>
-      <c r="B7" s="2">
-        <v>2.66479830114691E-5</v>
-      </c>
-      <c r="C7" s="2">
-        <v>9.0065523934370904E-5</v>
+      <c r="B7" s="1">
+        <v>2.6654638941437701E-5</v>
+      </c>
+      <c r="C7" s="1">
+        <v>9.0063449359562697E-5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>50.8</v>
       </c>
-      <c r="B8" s="2">
-        <v>2.92066847335379E-5</v>
-      </c>
-      <c r="C8" s="2">
-        <v>8.7506822212269703E-5</v>
+      <c r="B8" s="1">
+        <v>2.9222454639401802E-5</v>
+      </c>
+      <c r="C8" s="1">
+        <v>8.7495633661556794E-5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>59.266666666666701</v>
       </c>
-      <c r="B9" s="2">
-        <v>3.5313787672193602E-5</v>
-      </c>
-      <c r="C9" s="2">
-        <v>8.1399719273495702E-5</v>
+      <c r="B9" s="1">
+        <v>3.5347819780364603E-5</v>
+      </c>
+      <c r="C9" s="1">
+        <v>8.1370268520449503E-5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>67.733333333333306</v>
       </c>
-      <c r="B10" s="2">
-        <v>4.7152616168594397E-5</v>
-      </c>
-      <c r="C10" s="2">
-        <v>6.9560890776762605E-5</v>
+      <c r="B10" s="1">
+        <v>4.7212620373751401E-5</v>
+      </c>
+      <c r="C10" s="1">
+        <v>6.9505467926688004E-5</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>76.2</v>
       </c>
-      <c r="B11" s="2">
-        <v>6.4428228194754597E-5</v>
-      </c>
-      <c r="C11" s="2">
-        <v>5.2285278749964603E-5</v>
+      <c r="B11" s="1">
+        <v>6.4505443200368705E-5</v>
+      </c>
+      <c r="C11" s="1">
+        <v>5.2212645099457997E-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>